<commit_message>
Fix kickoff after PAT
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,10 +407,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ70"/>
+  <dimension ref="A1:AQ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -457,8 +457,8 @@
     <col customWidth="1" max="40" min="40" style="2" width="51.83203125"/>
     <col customWidth="1" max="41" min="41" style="2" width="23"/>
     <col customWidth="1" max="42" min="42" style="2" width="17"/>
-    <col customWidth="1" max="86" min="43" style="2" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="87" style="2" width="10.83203125"/>
+    <col customWidth="1" max="88" min="43" style="2" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="89" style="2" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1">
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H3" t="n">
         <v>3</v>
@@ -970,40 +970,40 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>2:37</t>
+          <t>0:37</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>James Madison 35</t>
+          <t>James Madison 20</t>
         </is>
       </c>
       <c r="AE3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF3" t="n">
         <v>10</v>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>James Madison</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>Hornet7Gaming#8204</t>
+          <t>door_nav#2953</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>KICKOFF</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>237</v>
+        <v>664</v>
       </c>
       <c r="AK3" t="n">
-        <v>923</v>
+        <v>1212</v>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="AQ3" t="inlineStr">
@@ -1218,70 +1218,6 @@
     </row>
     <row r="5"/>
     <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1335,8 +1271,8 @@
     <col customWidth="1" max="38" min="38" style="2" width="11.83203125"/>
     <col customWidth="1" max="39" min="39" style="2" width="12.83203125"/>
     <col customWidth="1" max="40" min="40" style="2" width="23.6640625"/>
-    <col customWidth="1" max="78" min="41" style="2" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="79" style="2" width="10.83203125"/>
+    <col customWidth="1" max="80" min="41" style="2" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="81" style="2" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1">

</xml_diff>

<commit_message>
Variety of bug fixes. Release of v1.0.1
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,7 +407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ6"/>
+  <dimension ref="A1:AQ71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
       <selection activeCell="AH3" sqref="AH3"/>
@@ -970,16 +970,16 @@
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>0:37</t>
+          <t>0:02</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>James Madison 20</t>
+          <t>James Madison 31</t>
         </is>
       </c>
       <c r="AE3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF3" t="n">
         <v>10</v>
@@ -1000,10 +1000,10 @@
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>664</v>
+        <v>444</v>
       </c>
       <c r="AK3" t="n">
-        <v>1212</v>
+        <v>5</v>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="AQ3" t="inlineStr">
@@ -1216,8 +1216,429 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>795451632363634688</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>South East North Western Wyoming A&amp;M Tech State</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Country Girls That Make Do</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PleaseEndMeNow#3186</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>spread</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>4-3</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>14</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>North Atlanta</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Hornets</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Starboy#1512</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>west coast</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Starboy#1512</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>defer</t>
+        </is>
+      </c>
+      <c r="AB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>0:38</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>South East North Western Wyoming A&amp;M Tech State 35</t>
+        </is>
+      </c>
+      <c r="AE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>South East North Western Wyoming A&amp;M Tech State</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>PleaseEndMeNow#3186</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>KICKOFF</t>
+        </is>
+      </c>
+      <c r="AJ5" t="n">
+        <v>555</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>45</v>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>PLAYING</t>
+        </is>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>2021/01/03/South East North Western Wyoming A&amp;M Tech State-vs-North Atlanta-795451632363634688</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>795451642782810132</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>795476008992112681</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mommy’s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Milkies</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>lancer52#4833</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>flexbone</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>5-2</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Milk University</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Milkmen</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Naki#2555</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>flexbone</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>4-4</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>7</v>
+      </c>
+      <c r="T6" t="n">
+        <v>3</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>lancer52#4833</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>defer</t>
+        </is>
+      </c>
+      <c r="AB6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>2:49</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Mommy’s 38</t>
+        </is>
+      </c>
+      <c r="AE6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>Milk University</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>Naki#2555</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="AJ6" t="n">
+        <v>378</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>597</v>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>PLAYING</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>2021/01/03/Mommy’s-vs-Milk University-795476008992112681</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>795476037051744267</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Variety of bug fixes.
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,7 +407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ71"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
       <selection activeCell="AH3" sqref="AH3"/>
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H3" t="n">
         <v>3</v>
@@ -966,23 +966,27 @@
         </is>
       </c>
       <c r="AB3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>0:02</t>
+          <t>6:15</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>James Madison 31</t>
-        </is>
-      </c>
-      <c r="AE3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>10</v>
+          <t>James Madison 30</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
@@ -1000,10 +1004,10 @@
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>444</v>
+        <v>33</v>
       </c>
       <c r="AK3" t="n">
-        <v>5</v>
+        <v>997</v>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
@@ -1027,7 +1031,7 @@
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="AQ3" t="inlineStr">
@@ -1248,7 +1252,7 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H5" t="n">
         <v>3</v>
@@ -1294,7 +1298,7 @@
         </is>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T5" t="n">
         <v>3</v>
@@ -1329,19 +1333,23 @@
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>0:38</t>
+          <t>0:15</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>South East North Western Wyoming A&amp;M Tech State 35</t>
-        </is>
-      </c>
-      <c r="AE5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>10</v>
+          <t>South East North Western Wyoming A&amp;M Tech State 25</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
@@ -1355,14 +1363,14 @@
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>KICKOFF</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="AJ5" t="n">
-        <v>555</v>
+        <v>777</v>
       </c>
       <c r="AK5" t="n">
-        <v>45</v>
+        <v>909</v>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
@@ -1508,137 +1516,252 @@
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>2:49</t>
+          <t>0:46</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>Mommy’s 38</t>
+          <t>Milk University 22</t>
         </is>
       </c>
       <c r="AE6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>Mommy’s</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>lancer52#4833</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="AJ6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>784</v>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>PLAYING</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>2021/01/03/Mommy’s-vs-Milk University-795476008992112681</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>795476037051744267</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>795506684675227668</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Footballers</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>JVitt#8369</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>air raid</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>4-4</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>USC</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Trojans</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>stinkywrestler#7847</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>spread</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>4-3</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>3</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="AB7" t="n">
         <v>1</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>Florida 35</t>
+        </is>
+      </c>
+      <c r="AE7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="n">
         <v>10</v>
       </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>Milk University</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>Naki#2555</t>
-        </is>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>NORMAL</t>
-        </is>
-      </c>
-      <c r="AJ6" t="n">
-        <v>378</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>597</v>
-      </c>
-      <c r="AL6" t="inlineStr">
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>JVitt#8369</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>KICKOFF</t>
+        </is>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL7" t="inlineStr">
         <is>
           <t>PLAYING</t>
         </is>
       </c>
-      <c r="AM6" t="inlineStr">
+      <c r="AM7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t>2021/01/03/Florida-vs-USC-795506684675227668</t>
+        </is>
+      </c>
+      <c r="AO7" t="inlineStr">
+        <is>
+          <t>795506691554672681</t>
+        </is>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AQ7" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="AN6" t="inlineStr">
-        <is>
-          <t>2021/01/03/Mommy’s-vs-Milk University-795476008992112681</t>
-        </is>
-      </c>
-      <c r="AO6" t="inlineStr">
-        <is>
-          <t>795476037051744267</t>
-        </is>
-      </c>
-      <c r="AP6" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="AQ6" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
-    <row r="7"/>
     <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Add config file and readme, as well as a gitignore
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,7 +407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ8"/>
+  <dimension ref="A1:AQ327"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
       <selection activeCell="AH3" sqref="AH3"/>
@@ -1043,27 +1043,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>794700021064138762</t>
+          <t>795451632363634688</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>South East North Western Wyoming A&amp;M Tech State</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nebraskans</t>
+          <t>Country Girls That Make Do</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hobbes .T. Hero#4989</t>
+          <t>PleaseEndMeNow#3186</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>pro</t>
+          <t>spread</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H4" t="n">
         <v>3</v>
@@ -1094,32 +1094,31 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>Gushbaba</t>
+          <t>North Atlanta</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Gushbabenbabens</t>
+          <t>Hornets</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Pizza Chef
-#2639</t>
+          <t>Starboy#1512</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>air raid</t>
+          <t>west coast</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="T4" t="n">
         <v>3</v>
@@ -1141,53 +1140,53 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>Starboy#1512</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>NONE</t>
+          <t>defer</t>
         </is>
       </c>
       <c r="AB4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>7:00</t>
+          <t>0:32</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>Nebraska 35</t>
+          <t>South East North Western Wyoming A&amp;M Tech State 28</t>
         </is>
       </c>
       <c r="AE4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AF4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>South East North Western Wyoming A&amp;M Tech State</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>Hobbes .T. Hero#4989</t>
+          <t>PleaseEndMeNow#3186</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>KICKOFF</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="AJ4" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="AK4" t="n">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
@@ -1196,63 +1195,63 @@
       </c>
       <c r="AM4" t="inlineStr">
         <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>2021/01/03/South East North Western Wyoming A&amp;M Tech State-vs-North Atlanta-795451632363634688</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>795451642782810132</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
           <t>YES</t>
-        </is>
-      </c>
-      <c r="AN4" t="inlineStr">
-        <is>
-          <t>2021/01/01/Nebraska-vs-Gushbaba-794700021064138762</t>
-        </is>
-      </c>
-      <c r="AO4" t="inlineStr">
-        <is>
-          <t>794700027112587305</t>
-        </is>
-      </c>
-      <c r="AP4" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="AQ4" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>795451632363634688</t>
+          <t>795476008992112681</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>South East North Western Wyoming A&amp;M Tech State</t>
+          <t>Mommy’s</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Country Girls That Make Do</t>
+          <t>Milkies</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PleaseEndMeNow#3186</t>
+          <t>lancer52#4833</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>spread</t>
+          <t>flexbone</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>5-2</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="H5" t="n">
         <v>3</v>
@@ -1274,27 +1273,27 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>North Atlanta</t>
+          <t>Milk University</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Hornets</t>
+          <t>Milkmen</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Starboy#1512</t>
+          <t>Naki#2555</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>west coast</t>
+          <t>flexbone</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>4-4</t>
         </is>
       </c>
       <c r="S5" t="n">
@@ -1320,7 +1319,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>Starboy#1512</t>
+          <t>lancer52#4833</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
@@ -1329,36 +1328,32 @@
         </is>
       </c>
       <c r="AB5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>3:22</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Mommy’s 30</t>
+        </is>
+      </c>
+      <c r="AE5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF5" t="n">
         <v>1</v>
       </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>0:15</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>South East North Western Wyoming A&amp;M Tech State 25</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>South East North Western Wyoming A&amp;M Tech State</t>
+          <t>Milk University</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>PleaseEndMeNow#3186</t>
+          <t>Naki#2555</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
@@ -1367,10 +1362,10 @@
         </is>
       </c>
       <c r="AJ5" t="n">
-        <v>777</v>
+        <v>290</v>
       </c>
       <c r="AK5" t="n">
-        <v>909</v>
+        <v>280</v>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
@@ -1379,17 +1374,17 @@
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>2021/01/03/South East North Western Wyoming A&amp;M Tech State-vs-North Atlanta-795451632363634688</t>
+          <t>2021/01/03/Mommy’s-vs-Milk University-795476008992112681</t>
         </is>
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>795451642782810132</t>
+          <t>795476037051744267</t>
         </is>
       </c>
       <c r="AP5" t="inlineStr">
@@ -1406,32 +1401,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>795476008992112681</t>
+          <t>795506684675227668</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mommy’s</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Milkies</t>
+          <t>Footballers</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>lancer52#4833</t>
+          <t>JVitt#8369</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>flexbone</t>
+          <t>air raid</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>5-2</t>
+          <t>4-4</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -1457,27 +1452,27 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Milk University</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Milkmen</t>
+          <t>Trojans</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Naki#2555</t>
+          <t>stinkywrestler#7847</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>flexbone</t>
+          <t>spread</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="S6" t="n">
@@ -1503,7 +1498,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>lancer52#4833</t>
+          <t>stinkywrestler#7847</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
@@ -1512,32 +1507,32 @@
         </is>
       </c>
       <c r="AB6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>6:31</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Florida 29</t>
+        </is>
+      </c>
+      <c r="AE6" t="n">
         <v>1</v>
       </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>0:46</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>Milk University 22</t>
-        </is>
-      </c>
-      <c r="AE6" t="n">
-        <v>2</v>
-      </c>
       <c r="AF6" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>Mommy’s</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>lancer52#4833</t>
+          <t>JVitt#8369</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
@@ -1546,10 +1541,10 @@
         </is>
       </c>
       <c r="AJ6" t="n">
-        <v>1000</v>
+        <v>777</v>
       </c>
       <c r="AK6" t="n">
-        <v>784</v>
+        <v>999</v>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
@@ -1558,22 +1553,22 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>2021/01/03/Mommy’s-vs-Milk University-795476008992112681</t>
+          <t>2021/01/03/Florida-vs-USC-795506684675227668</t>
         </is>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>795476037051744267</t>
+          <t>795506691554672681</t>
         </is>
       </c>
       <c r="AP6" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="AQ6" t="inlineStr">
@@ -1585,22 +1580,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>795506684675227668</t>
+          <t>795731302955089941</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Footballers</t>
+          <t>Nebraskans</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>JVitt#8369</t>
+          <t>Hobbes .T. Hero#4989</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1610,7 +1605,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -1636,22 +1631,22 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Gushbaba</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Trojans</t>
+          <t>Gushbabenbabens</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>stinkywrestler#7847</t>
+          <t>Pizza Chef#2639</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>spread</t>
+          <t>air raid</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1700,7 +1695,7 @@
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>Florida 35</t>
+          <t>Nebraska 35</t>
         </is>
       </c>
       <c r="AE7" t="n">
@@ -1711,12 +1706,12 @@
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>JVitt#8369</t>
+          <t>Hobbes .T. Hero#4989</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
@@ -1742,12 +1737,12 @@
       </c>
       <c r="AN7" t="inlineStr">
         <is>
-          <t>2021/01/03/Florida-vs-USC-795506684675227668</t>
+          <t>2021/01/04/Nebraska-vs-Gushbaba-795731302955089941</t>
         </is>
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>795506691554672681</t>
+          <t>795731307208507422</t>
         </is>
       </c>
       <c r="AP7" t="inlineStr">
@@ -1762,6 +1757,325 @@
       </c>
     </row>
     <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
+    <row r="247"/>
+    <row r="248"/>
+    <row r="249"/>
+    <row r="250"/>
+    <row r="251"/>
+    <row r="252"/>
+    <row r="253"/>
+    <row r="254"/>
+    <row r="255"/>
+    <row r="256"/>
+    <row r="257"/>
+    <row r="258"/>
+    <row r="259"/>
+    <row r="260"/>
+    <row r="261"/>
+    <row r="262"/>
+    <row r="263"/>
+    <row r="264"/>
+    <row r="265"/>
+    <row r="266"/>
+    <row r="267"/>
+    <row r="268"/>
+    <row r="269"/>
+    <row r="270"/>
+    <row r="271"/>
+    <row r="272"/>
+    <row r="273"/>
+    <row r="274"/>
+    <row r="275"/>
+    <row r="276"/>
+    <row r="277"/>
+    <row r="278"/>
+    <row r="279"/>
+    <row r="280"/>
+    <row r="281"/>
+    <row r="282"/>
+    <row r="283"/>
+    <row r="284"/>
+    <row r="285"/>
+    <row r="286"/>
+    <row r="287"/>
+    <row r="288"/>
+    <row r="289"/>
+    <row r="290"/>
+    <row r="291"/>
+    <row r="292"/>
+    <row r="293"/>
+    <row r="294"/>
+    <row r="295"/>
+    <row r="296"/>
+    <row r="297"/>
+    <row r="298"/>
+    <row r="299"/>
+    <row r="300"/>
+    <row r="301"/>
+    <row r="302"/>
+    <row r="303"/>
+    <row r="304"/>
+    <row r="305"/>
+    <row r="306"/>
+    <row r="307"/>
+    <row r="308"/>
+    <row r="309"/>
+    <row r="310"/>
+    <row r="311"/>
+    <row r="312"/>
+    <row r="313"/>
+    <row r="314"/>
+    <row r="315"/>
+    <row r="316"/>
+    <row r="317"/>
+    <row r="318"/>
+    <row r="319"/>
+    <row r="320"/>
+    <row r="321"/>
+    <row r="322"/>
+    <row r="323"/>
+    <row r="324"/>
+    <row r="325"/>
+    <row r="326"/>
+    <row r="327"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Delete log file on command
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apkick/Documents/Programming/FCFB-Ref-Bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1D7E6E-6952-B248-A0EB-7A8F714F4B28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F6CCCF-B4D8-D94B-975B-EC313BB65779}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="127">
   <si>
     <t>Channel ID</t>
   </si>
@@ -188,223 +188,220 @@
     <t>3:44</t>
   </si>
   <si>
-    <t>Utah 35</t>
+    <t>Philadelphia 25</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>PLAYING</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>2021/01/01/Philadelphia-vs-Utah-794629920688046080</t>
+  </si>
+  <si>
+    <t>794629926140641280</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>794683644382806096</t>
+  </si>
+  <si>
+    <t>Omaha</t>
+  </si>
+  <si>
+    <t>Settlers</t>
+  </si>
+  <si>
+    <t>Hornet7Gaming#8204</t>
+  </si>
+  <si>
+    <t>spread</t>
+  </si>
+  <si>
+    <t>4-4</t>
+  </si>
+  <si>
+    <t>James Madison</t>
+  </si>
+  <si>
+    <t>Dukes</t>
+  </si>
+  <si>
+    <t>door_nav#2953</t>
+  </si>
+  <si>
+    <t>defer</t>
+  </si>
+  <si>
+    <t>2021/01/01/Omaha-vs-James Madison-794683644382806096</t>
+  </si>
+  <si>
+    <t>794683648585891870</t>
+  </si>
+  <si>
+    <t>795451632363634688</t>
+  </si>
+  <si>
+    <t>South East North Western Wyoming A&amp;M Tech State</t>
+  </si>
+  <si>
+    <t>Country Girls That Make Do</t>
+  </si>
+  <si>
+    <t>PleaseEndMeNow#3186</t>
+  </si>
+  <si>
+    <t>North Atlanta</t>
+  </si>
+  <si>
+    <t>Hornets</t>
+  </si>
+  <si>
+    <t>Starboy#1512</t>
+  </si>
+  <si>
+    <t>west coast</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>0:32</t>
+  </si>
+  <si>
+    <t>South East North Western Wyoming A&amp;M Tech State 28</t>
+  </si>
+  <si>
+    <t>2021/01/03/South East North Western Wyoming A&amp;M Tech State-vs-North Atlanta-795451632363634688</t>
+  </si>
+  <si>
+    <t>795451642782810132</t>
+  </si>
+  <si>
+    <t>795476008992112681</t>
+  </si>
+  <si>
+    <t>Mommy’s</t>
+  </si>
+  <si>
+    <t>Milkies</t>
+  </si>
+  <si>
+    <t>lancer52#4833</t>
+  </si>
+  <si>
+    <t>5-2</t>
+  </si>
+  <si>
+    <t>Milk University</t>
+  </si>
+  <si>
+    <t>Milkmen</t>
+  </si>
+  <si>
+    <t>Naki#2555</t>
+  </si>
+  <si>
+    <t>3:22</t>
+  </si>
+  <si>
+    <t>Mommy’s 30</t>
+  </si>
+  <si>
+    <t>2021/01/03/Mommy’s-vs-Milk University-795476008992112681</t>
+  </si>
+  <si>
+    <t>795476037051744267</t>
+  </si>
+  <si>
+    <t>795506684675227668</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Footballers</t>
+  </si>
+  <si>
+    <t>JVitt#8369</t>
+  </si>
+  <si>
+    <t>air raid</t>
+  </si>
+  <si>
+    <t>USC</t>
+  </si>
+  <si>
+    <t>Trojans</t>
+  </si>
+  <si>
+    <t>stinkywrestler#7847</t>
+  </si>
+  <si>
+    <t>6:31</t>
+  </si>
+  <si>
+    <t>USC 29</t>
+  </si>
+  <si>
+    <t>2021/01/03/Florida-vs-USC-795506684675227668</t>
+  </si>
+  <si>
+    <t>795506691554672681</t>
+  </si>
+  <si>
+    <t>795731302955089941</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nebraskans</t>
+  </si>
+  <si>
+    <t>Hobbes .T. Hero#4989</t>
+  </si>
+  <si>
+    <t>Gushbaba</t>
+  </si>
+  <si>
+    <t>Gushbabenbabens</t>
+  </si>
+  <si>
+    <t>Pizza Chef#2639</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>Nebraska 35</t>
   </si>
   <si>
     <t>KICKOFF</t>
   </si>
   <si>
-    <t>PLAYING</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>2021/01/01/Philadelphia-vs-Utah-794629920688046080</t>
-  </si>
-  <si>
-    <t>794629926140641280</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>794683644382806096</t>
-  </si>
-  <si>
-    <t>Omaha</t>
-  </si>
-  <si>
-    <t>Settlers</t>
-  </si>
-  <si>
-    <t>Hornet7Gaming#8204</t>
-  </si>
-  <si>
-    <t>spread</t>
-  </si>
-  <si>
-    <t>4-4</t>
-  </si>
-  <si>
-    <t>James Madison</t>
-  </si>
-  <si>
-    <t>Dukes</t>
-  </si>
-  <si>
-    <t>door_nav#2953</t>
-  </si>
-  <si>
-    <t>defer</t>
-  </si>
-  <si>
-    <t>6:15</t>
+    <t>2021/01/04/Nebraska-vs-Gushbaba-795731302955089941</t>
+  </si>
+  <si>
+    <t>795731307208507422</t>
   </si>
   <si>
     <t>James Madison 30</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>NORMAL</t>
-  </si>
-  <si>
-    <t>2021/01/01/Omaha-vs-James Madison-794683644382806096</t>
-  </si>
-  <si>
-    <t>794683648585891870</t>
-  </si>
-  <si>
-    <t>795451632363634688</t>
-  </si>
-  <si>
-    <t>South East North Western Wyoming A&amp;M Tech State</t>
-  </si>
-  <si>
-    <t>Country Girls That Make Do</t>
-  </si>
-  <si>
-    <t>PleaseEndMeNow#3186</t>
-  </si>
-  <si>
-    <t>North Atlanta</t>
-  </si>
-  <si>
-    <t>Hornets</t>
-  </si>
-  <si>
-    <t>Starboy#1512</t>
-  </si>
-  <si>
-    <t>west coast</t>
-  </si>
-  <si>
-    <t>3-4</t>
-  </si>
-  <si>
-    <t>0:32</t>
-  </si>
-  <si>
-    <t>South East North Western Wyoming A&amp;M Tech State 28</t>
-  </si>
-  <si>
-    <t>2021/01/03/South East North Western Wyoming A&amp;M Tech State-vs-North Atlanta-795451632363634688</t>
-  </si>
-  <si>
-    <t>795451642782810132</t>
-  </si>
-  <si>
-    <t>795476008992112681</t>
-  </si>
-  <si>
-    <t>Mommy’s</t>
-  </si>
-  <si>
-    <t>Milkies</t>
-  </si>
-  <si>
-    <t>lancer52#4833</t>
-  </si>
-  <si>
-    <t>5-2</t>
-  </si>
-  <si>
-    <t>Milk University</t>
-  </si>
-  <si>
-    <t>Milkmen</t>
-  </si>
-  <si>
-    <t>Naki#2555</t>
-  </si>
-  <si>
-    <t>3:22</t>
-  </si>
-  <si>
-    <t>Mommy’s 30</t>
-  </si>
-  <si>
-    <t>2021/01/03/Mommy’s-vs-Milk University-795476008992112681</t>
-  </si>
-  <si>
-    <t>795476037051744267</t>
-  </si>
-  <si>
-    <t>795506684675227668</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Footballers</t>
-  </si>
-  <si>
-    <t>JVitt#8369</t>
-  </si>
-  <si>
-    <t>air raid</t>
-  </si>
-  <si>
-    <t>USC</t>
-  </si>
-  <si>
-    <t>Trojans</t>
-  </si>
-  <si>
-    <t>stinkywrestler#7847</t>
-  </si>
-  <si>
-    <t>6:31</t>
-  </si>
-  <si>
-    <t>2021/01/03/Florida-vs-USC-795506684675227668</t>
-  </si>
-  <si>
-    <t>795506691554672681</t>
-  </si>
-  <si>
-    <t>795731302955089941</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Nebraskans</t>
-  </si>
-  <si>
-    <t>Hobbes .T. Hero#4989</t>
-  </si>
-  <si>
-    <t>Gushbaba</t>
-  </si>
-  <si>
-    <t>Gushbabenbabens</t>
-  </si>
-  <si>
-    <t>Pizza Chef#2639</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>7:00</t>
-  </si>
-  <si>
-    <t>Nebraska 35</t>
-  </si>
-  <si>
-    <t>2021/01/04/Nebraska-vs-Gushbaba-795731302955089941</t>
-  </si>
-  <si>
-    <t>795731307208507422</t>
-  </si>
-  <si>
-    <t>USC 29</t>
   </si>
 </sst>
 </file>
@@ -453,11 +450,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:CK7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,11 +786,11 @@
     <col min="40" max="40" width="51.83203125" style="2" customWidth="1"/>
     <col min="41" max="41" width="23" style="2" customWidth="1"/>
     <col min="42" max="42" width="17" style="2" customWidth="1"/>
-    <col min="43" max="89" width="10.83203125" style="2" customWidth="1"/>
-    <col min="90" max="16384" width="10.83203125" style="2"/>
+    <col min="43" max="90" width="10.83203125" style="2" customWidth="1"/>
+    <col min="91" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:89" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +921,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:89" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1014,11 +1012,11 @@
       <c r="AD2" t="s">
         <v>55</v>
       </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>10</v>
+      <c r="AE2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>57</v>
       </c>
       <c r="AG2" t="s">
         <v>44</v>
@@ -1027,51 +1025,51 @@
         <v>46</v>
       </c>
       <c r="AI2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AJ2">
-        <v>616</v>
+        <v>250</v>
       </c>
       <c r="AK2">
-        <v>36</v>
+        <v>250</v>
       </c>
       <c r="AL2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AM2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AN2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AO2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP2" t="s">
         <v>60</v>
       </c>
-      <c r="AP2" t="s">
-        <v>58</v>
-      </c>
       <c r="AQ2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>62</v>
+    <row r="3" spans="1:89" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="G3">
         <v>14</v>
@@ -1095,19 +1093,19 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" t="s">
         <v>68</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="P3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" t="s">
-        <v>67</v>
       </c>
       <c r="S3">
         <v>14</v>
@@ -1131,34 +1129,34 @@
         <v>0</v>
       </c>
       <c r="Z3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AA3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AB3">
         <v>2</v>
       </c>
-      <c r="AC3" t="s">
-        <v>72</v>
+      <c r="AC3" s="4">
+        <v>0.26041666666666669</v>
       </c>
       <c r="AD3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>75</v>
+        <v>126</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>10</v>
       </c>
       <c r="AG3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AH3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AI3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="AJ3">
         <v>33</v>
@@ -1167,39 +1165,85 @@
         <v>997</v>
       </c>
       <c r="AL3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AM3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AN3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR3"/>
+      <c r="AS3"/>
+      <c r="AT3"/>
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+      <c r="BA3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
+      <c r="BD3"/>
+      <c r="BE3"/>
+      <c r="BF3"/>
+      <c r="BG3"/>
+      <c r="BH3"/>
+      <c r="BI3"/>
+      <c r="BJ3"/>
+      <c r="BK3"/>
+      <c r="BL3"/>
+      <c r="BM3"/>
+      <c r="BN3"/>
+      <c r="BO3"/>
+      <c r="BP3"/>
+      <c r="BQ3"/>
+      <c r="BR3"/>
+      <c r="BS3"/>
+      <c r="BT3"/>
+      <c r="BU3"/>
+      <c r="BV3"/>
+      <c r="BW3"/>
+      <c r="BX3"/>
+      <c r="BY3"/>
+      <c r="BZ3"/>
+      <c r="CA3"/>
+      <c r="CB3"/>
+      <c r="CC3"/>
+      <c r="CD3"/>
+      <c r="CE3"/>
+      <c r="CF3"/>
+      <c r="CG3"/>
+      <c r="CH3"/>
+      <c r="CI3"/>
+      <c r="CJ3"/>
+      <c r="CK3"/>
+    </row>
+    <row r="4" spans="1:89" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
         <v>77</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="C4" t="s">
         <v>78</v>
       </c>
-      <c r="AP3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>79</v>
       </c>
-      <c r="B4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" t="s">
-        <v>82</v>
-      </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F4" t="s">
         <v>48</v>
@@ -1226,19 +1270,19 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q4" t="s">
         <v>83</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>84</v>
-      </c>
-      <c r="P4" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>86</v>
-      </c>
-      <c r="R4" t="s">
-        <v>87</v>
       </c>
       <c r="S4">
         <v>28</v>
@@ -1262,19 +1306,19 @@
         <v>0</v>
       </c>
       <c r="Z4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AA4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AB4">
         <v>2</v>
       </c>
       <c r="AC4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AD4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="AE4">
         <v>4</v>
@@ -1283,13 +1327,13 @@
         <v>7</v>
       </c>
       <c r="AG4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="AH4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AI4" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="AJ4">
         <v>42</v>
@@ -1298,42 +1342,42 @@
         <v>1200</v>
       </c>
       <c r="AL4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AM4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AN4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:89" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="C5" t="s">
         <v>91</v>
       </c>
-      <c r="AP4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" t="s">
-        <v>95</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -1357,19 +1401,19 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="O5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="P5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q5" t="s">
         <v>47</v>
       </c>
       <c r="R5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S5">
         <v>7</v>
@@ -1393,19 +1437,19 @@
         <v>0</v>
       </c>
       <c r="Z5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AA5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AB5">
         <v>2</v>
       </c>
       <c r="AC5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="AD5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="AE5">
         <v>4</v>
@@ -1414,13 +1458,13 @@
         <v>1</v>
       </c>
       <c r="AG5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AH5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="AI5" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="AJ5">
         <v>290</v>
@@ -1429,42 +1473,42 @@
         <v>280</v>
       </c>
       <c r="AL5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AM5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AN5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:89" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
         <v>102</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="C6" t="s">
         <v>103</v>
       </c>
-      <c r="AP5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
         <v>104</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>105</v>
       </c>
-      <c r="C6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" t="s">
-        <v>108</v>
-      </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1488,16 +1532,16 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="P6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R6" t="s">
         <v>48</v>
@@ -1524,19 +1568,19 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AA6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AB6">
         <v>2</v>
       </c>
       <c r="AC6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AD6" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="AE6">
         <v>1</v>
@@ -1545,13 +1589,13 @@
         <v>10</v>
       </c>
       <c r="AG6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AH6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="AI6" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="AJ6">
         <v>777</v>
@@ -1560,39 +1604,39 @@
         <v>999</v>
       </c>
       <c r="AL6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AM6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AN6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:89" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>113</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="B7" t="s">
         <v>114</v>
       </c>
-      <c r="AP6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>115</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>116</v>
       </c>
-      <c r="C7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D7" t="s">
-        <v>118</v>
-      </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
         <v>48</v>
@@ -1619,16 +1663,16 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O7" t="s">
+        <v>118</v>
+      </c>
+      <c r="P7" t="s">
         <v>119</v>
       </c>
-      <c r="O7" t="s">
-        <v>120</v>
-      </c>
-      <c r="P7" t="s">
-        <v>121</v>
-      </c>
       <c r="Q7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="R7" t="s">
         <v>48</v>
@@ -1655,19 +1699,19 @@
         <v>0</v>
       </c>
       <c r="Z7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AA7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AB7">
         <v>1</v>
       </c>
       <c r="AC7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AD7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="AE7">
         <v>1</v>
@@ -1676,13 +1720,13 @@
         <v>10</v>
       </c>
       <c r="AG7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH7" t="s">
         <v>116</v>
       </c>
-      <c r="AH7" t="s">
-        <v>118</v>
-      </c>
       <c r="AI7" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="AJ7">
         <v>0</v>
@@ -1691,22 +1735,22 @@
         <v>0</v>
       </c>
       <c r="AL7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AM7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AN7" t="s">
+        <v>124</v>
+      </c>
+      <c r="AO7" t="s">
         <v>125</v>
       </c>
-      <c r="AO7" t="s">
-        <v>126</v>
-      </c>
       <c r="AP7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AQ7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1758,8 +1802,8 @@
     <col min="38" max="38" width="11.83203125" style="2" customWidth="1"/>
     <col min="39" max="39" width="12.83203125" style="2" customWidth="1"/>
     <col min="40" max="40" width="23.6640625" style="2" customWidth="1"/>
-    <col min="41" max="81" width="10.83203125" style="2" customWidth="1"/>
-    <col min="82" max="16384" width="10.83203125" style="2"/>
+    <col min="41" max="82" width="10.83203125" style="2" customWidth="1"/>
+    <col min="83" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add new ranges and a way to track them
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,7 +407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ9"/>
+  <dimension ref="A1:AQ91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <selection activeCell="AC4" sqref="AC4"/>
@@ -1621,7 +1621,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H7" t="n">
         <v>3</v>
@@ -1702,32 +1702,28 @@
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>4:49</t>
+          <t>0:27</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>Gushbaba 7</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+          <t>Gushbaba 37</t>
+        </is>
+      </c>
+      <c r="AE7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>10</v>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>Gushbaba</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>Pizza Chef#2639</t>
+          <t>Hobbes .T. Hero#4989</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
@@ -1739,7 +1735,7 @@
         <v>750</v>
       </c>
       <c r="AK7" t="n">
-        <v>1489</v>
+        <v>1201</v>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
@@ -1774,6 +1770,88 @@
     </row>
     <row r="8"/>
     <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fixes and more error messages
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,10 +407,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ11"/>
+  <dimension ref="A1:AQ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -458,8 +458,8 @@
     <col bestFit="1" customWidth="1" max="41" min="41" style="2" width="19.33203125"/>
     <col customWidth="1" max="42" min="42" style="2" width="17"/>
     <col bestFit="1" customWidth="1" max="43" min="43" style="2" width="8.33203125"/>
-    <col customWidth="1" max="98" min="44" style="2" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="99" style="2" width="10.83203125"/>
+    <col customWidth="1" max="99" min="44" style="2" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="100" style="2" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="S3" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T3" t="n">
         <v>3</v>
@@ -976,7 +976,7 @@
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>Omaha 3</t>
+          <t>James Madison 35</t>
         </is>
       </c>
       <c r="AE3" t="n">
@@ -997,11 +997,11 @@
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>TOUCHDOWN</t>
+          <t>KICKOFF</t>
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>1002</v>
+        <v>665</v>
       </c>
       <c r="AK3" t="n">
         <v>1001</v>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="AQ3" t="inlineStr">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PleaseEndMeNow#3186</t>
+          <t>Buttersqauch#3186</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>PleaseEndMeNow#3186</t>
+          <t>Buttersqauch#3186</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
@@ -1187,7 +1187,7 @@
         <v>545</v>
       </c>
       <c r="AK4" t="n">
-        <v>1278</v>
+        <v>55</v>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="AQ4" t="inlineStr">
@@ -1766,9 +1766,6 @@
       </c>
     </row>
     <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1822,8 +1819,8 @@
     <col customWidth="1" max="38" min="38" style="2" width="11.83203125"/>
     <col customWidth="1" max="39" min="39" style="2" width="12.83203125"/>
     <col customWidth="1" max="40" min="40" style="2" width="23.6640625"/>
-    <col customWidth="1" max="90" min="41" style="2" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="91" style="2" width="10.83203125"/>
+    <col customWidth="1" max="91" min="41" style="2" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="92" style="2" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1">

</xml_diff>

<commit_message>
Bunch of bug fixes like turnovers and field goal field position
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,10 +407,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ8"/>
+  <dimension ref="A1:AQ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AP3" sqref="AP3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -458,8 +458,8 @@
     <col bestFit="1" customWidth="1" max="41" min="41" style="2" width="19.33203125"/>
     <col customWidth="1" max="42" min="42" style="2" width="17"/>
     <col bestFit="1" customWidth="1" max="43" min="43" style="2" width="8.33203125"/>
-    <col customWidth="1" max="99" min="44" style="2" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="100" style="2" width="10.83203125"/>
+    <col customWidth="1" max="113" min="44" style="2" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="114" style="2" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1">
@@ -967,44 +967,44 @@
         </is>
       </c>
       <c r="AB3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="2" t="inlineStr">
+        <is>
+          <t>6:55</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>Omaha 29</t>
+        </is>
+      </c>
+      <c r="AE3" t="n">
         <v>2</v>
       </c>
-      <c r="AC3" s="2" t="inlineStr">
-        <is>
-          <t>0:56</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>James Madison 35</t>
-        </is>
-      </c>
-      <c r="AE3" t="n">
+      <c r="AF3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>Omaha</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>door_nav#2953</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="AJ3" t="n">
         <v>1</v>
       </c>
-      <c r="AF3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>James Madison</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>door_nav#2953</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>KICKOFF</t>
-        </is>
-      </c>
-      <c r="AJ3" t="n">
-        <v>665</v>
-      </c>
       <c r="AK3" t="n">
-        <v>1001</v>
+        <v>333</v>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="AN3" t="inlineStr">
@@ -1148,46 +1148,42 @@
       <c r="AB4" t="n">
         <v>3</v>
       </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>7:00</t>
+      <c r="AC4" s="2" t="inlineStr">
+        <is>
+          <t>6:52</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>South East North Western Wyoming A&amp;M Tech State 17</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+          <t>South East North Western Wyoming A&amp;M Tech State 45</t>
+        </is>
+      </c>
+      <c r="AE4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>10</v>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>South East North Western Wyoming A&amp;M Tech State</t>
+          <t>North Atlanta</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>Buttersqauch#3186</t>
+          <t>Starboy#1512</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>KICKOFF</t>
+          <t>NORMAL</t>
         </is>
       </c>
       <c r="AJ4" t="n">
-        <v>545</v>
+        <v>720</v>
       </c>
       <c r="AK4" t="n">
-        <v>55</v>
+        <v>1138</v>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
@@ -1211,7 +1207,7 @@
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="AQ4" t="inlineStr">
@@ -1358,7 +1354,7 @@
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>lancer52#4833</t>
+          <t>Naki#2555</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
@@ -1481,7 +1477,7 @@
         </is>
       </c>
       <c r="S6" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="T6" t="n">
         <v>3</v>
@@ -1516,32 +1512,28 @@
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>4:13</t>
+          <t>2:05</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>Florida 20</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+          <t>USC 33</t>
+        </is>
+      </c>
+      <c r="AE6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>10</v>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>JVitt#8369</t>
+          <t>stinkywrestler#7847</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
@@ -1550,10 +1542,10 @@
         </is>
       </c>
       <c r="AJ6" t="n">
-        <v>222</v>
+        <v>992</v>
       </c>
       <c r="AK6" t="n">
-        <v>751</v>
+        <v>661</v>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
@@ -1765,7 +1757,192 @@
         </is>
       </c>
     </row>
-    <row r="8"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>798042930433884191</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>springfield</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Springs</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Turts#3627</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>air raid</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>4-4</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>14</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>UMKC</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>‘Roos</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>KOZ#1949</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>spread</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>4-3</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>3</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>Turts#3627</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>defer</t>
+        </is>
+      </c>
+      <c r="AB8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>1:31</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>springfield 35</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>UMKC</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>KOZ#1949</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="AJ8" t="n">
+        <v>761</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>671</v>
+      </c>
+      <c r="AL8" t="inlineStr">
+        <is>
+          <t>PLAYING</t>
+        </is>
+      </c>
+      <c r="AM8" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AN8" t="inlineStr">
+        <is>
+          <t>2021/01/11/springfield-vs-UMKC-798042930433884191</t>
+        </is>
+      </c>
+      <c r="AO8" t="inlineStr">
+        <is>
+          <t>798042935563255848</t>
+        </is>
+      </c>
+      <c r="AP8" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AQ8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1777,7 +1954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN9"/>
+  <dimension ref="A1:AO9"/>
   <sheetViews>
     <sheetView topLeftCell="AJ1" workbookViewId="0">
       <selection activeCell="AN1" sqref="AN1"/>
@@ -1819,8 +1996,8 @@
     <col customWidth="1" max="38" min="38" style="2" width="11.83203125"/>
     <col customWidth="1" max="39" min="39" style="2" width="12.83203125"/>
     <col customWidth="1" max="40" min="40" style="2" width="23.6640625"/>
-    <col customWidth="1" max="91" min="41" style="2" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="92" style="2" width="10.83203125"/>
+    <col customWidth="1" max="105" min="41" style="2" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="106" style="2" width="10.83203125"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1">
@@ -2022,6 +2199,344 @@
       <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Gist Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>796942741086273556</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cudahy</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Chuds</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>penguino#2114</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>air raid</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>5-2</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Springfield</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Springs</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Turts#3627</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>air raid</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>4-4</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>3</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>penguino#2114</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>defer</t>
+        </is>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>6:36</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Springfield 17</t>
+        </is>
+      </c>
+      <c r="AE2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>Springfield</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>penguino#2114</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>NORMAL</t>
+        </is>
+      </c>
+      <c r="AJ2" t="n">
+        <v>69</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1212</v>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>PLAYING</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>2021/01/07/Cudahy-vs-Springfield-796942741086273556</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>796942747129872405</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>796954332461006888</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cudahy</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chuds</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>penguino#2114</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>air raid</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5-2</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>184</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>springfield</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Springs</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Turts#3627</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>air raid</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>4-4</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>64</v>
+      </c>
+      <c r="T3" t="n">
+        <v>3</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Turts#3627</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>defer</t>
+        </is>
+      </c>
+      <c r="AB3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>7:00</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>springfield 35</t>
+        </is>
+      </c>
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>springfield</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>penguino#2114</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>GAME DONE</t>
+        </is>
+      </c>
+      <c r="AJ3" t="n">
+        <v>69</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>751</v>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>FINISHED</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>2021/01/07/cudahy-vs-springfield-796954332461006888</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>796954339955572766</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix issue regarding an error when FCFB Ref Bot sent a DM
</commit_message>
<xml_diff>
--- a/game_database.xlsx
+++ b/game_database.xlsx
@@ -407,7 +407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ11"/>
+  <dimension ref="A1:AQ12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
       <selection activeCell="AP3" sqref="AP3"/>
@@ -971,19 +971,19 @@
       </c>
       <c r="AC3" s="2" t="inlineStr">
         <is>
-          <t>6:55</t>
+          <t>6:21</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>Omaha 29</t>
+          <t>Omaha 30</t>
         </is>
       </c>
       <c r="AE3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AF3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
@@ -1001,10 +1001,10 @@
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="AK3" t="n">
-        <v>333</v>
+        <v>1221</v>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
@@ -1943,6 +1943,7 @@
     <row r="9"/>
     <row r="10"/>
     <row r="11"/>
+    <row r="12"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>